<commit_message>
Added Excel import modules as examples
</commit_message>
<xml_diff>
--- a/python-client/examples/excel_example_hrm.xlsx
+++ b/python-client/examples/excel_example_hrm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jryi/dev/aava-api-integrations/python-client/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jryi/dev/aava-api-integrations/python-client/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD8FAB2D-E8AD-F54B-898D-B7BF9E21C1CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8C27C3-1C18-194E-8065-E8B7C2BC18EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21060" yWindow="10980" windowWidth="28040" windowHeight="17440" xr2:uid="{6B3185BA-B712-6247-A6E2-50F76BEAD79E}"/>
+    <workbookView xWindow="1220" yWindow="9900" windowWidth="28040" windowHeight="17440" xr2:uid="{6B3185BA-B712-6247-A6E2-50F76BEAD79E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>externalId</t>
   </si>
@@ -82,6 +82,66 @@
   </si>
   <si>
     <t>supervisorStart</t>
+  </si>
+  <si>
+    <t>ceo</t>
+  </si>
+  <si>
+    <t>emp1</t>
+  </si>
+  <si>
+    <t>emp2</t>
+  </si>
+  <si>
+    <t>090977-954P</t>
+  </si>
+  <si>
+    <t>161165-951M</t>
+  </si>
+  <si>
+    <t>110674-9046</t>
+  </si>
+  <si>
+    <t>Cecily</t>
+  </si>
+  <si>
+    <t>Ceo</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Ant</t>
+  </si>
+  <si>
+    <t>Betty</t>
+  </si>
+  <si>
+    <t>Boo</t>
+  </si>
+  <si>
+    <t>ceo@company.com</t>
+  </si>
+  <si>
+    <t>adam.ant@company.com</t>
+  </si>
+  <si>
+    <t>betty.boo@company.com</t>
+  </si>
+  <si>
+    <t>0101234567</t>
+  </si>
+  <si>
+    <t>0101122334</t>
+  </si>
+  <si>
+    <t>0107654321</t>
+  </si>
+  <si>
+    <t>dep1</t>
+  </si>
+  <si>
+    <t>dep2</t>
   </si>
 </sst>
 </file>
@@ -125,9 +185,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,13 +505,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0641F75C-68AC-0148-ABDF-D4AC7FB504E9}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -498,6 +565,110 @@
       </c>
       <c r="P1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="4">
+        <v>42401</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="4">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4">
+        <v>43102</v>
+      </c>
+      <c r="L3" s="4">
+        <v>44196</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="4">
+        <v>43132</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="4">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="4">
+        <v>42767</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="4">
+        <v>42767</v>
+      </c>
+      <c r="O4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="4">
+        <v>42767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>